<commit_message>
More work on final Clemens comments
SIM showcase is a bit of a mess at the moment...
</commit_message>
<xml_diff>
--- a/pockels contrast figure/pockles voltage vs contrast.xlsx
+++ b/pockels contrast figure/pockles voltage vs contrast.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carcu\Documents\PhD\thesis\pockels contrast figure\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carcu\Documents\PhD\thesis 2\pockels contrast figure\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1500A04A-4C8E-425C-8312-1C18986EC7D5}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EBE7F4B-B89A-48A3-B45A-5E7074A56D7E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{C9D3B2A5-77B6-4088-9073-BD21F9E64163}"/>
   </bookViews>
@@ -16,10 +16,16 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -1397,7 +1403,1319 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Pattern contrast vs.</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" baseline="0"/>
+              <a:t> Pockels cell voltage for 561nm channel</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0°</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$A$2:$A$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="40"/>
+                <c:pt idx="0">
+                  <c:v>-375</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-355.76923076923089</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-336.53846153846177</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-317.30769230769226</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-298.07692307692315</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-278.84615384615398</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-259.61538461538447</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-240.38461538461536</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-221.15384615384625</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-201.92307692307674</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-182.69230769230762</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-163.46153846153851</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-144.2307692307694</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-124.99999999999987</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-105.76923076923075</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-86.538461538461632</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-67.307692307692491</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>-48.076923076923002</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>-28.846153846153836</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>-9.6153846153846363</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>9.615384615384599</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>28.846153846153836</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>48.076923076923002</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>67.307692307692491</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>86.538461538461632</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>105.76923076923075</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>124.99999999999987</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>144.2307692307694</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>163.46153846153851</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>182.69230769230762</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>201.92307692307713</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>221.15384615384625</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>240.38461538461536</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>259.61538461538447</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>278.84615384615398</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>298.07692307692315</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>317.30769230769226</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>336.53846153846138</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>355.76923076923089</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>375</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$F$2:$F$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="40"/>
+                <c:pt idx="0">
+                  <c:v>0.93460750664971581</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.88921086627950874</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.80895359754091334</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.70382335956106368</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.5970662829615776</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.48301577109411531</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.38254029659280375</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.27416444981191507</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.19902187846008601</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.14272764542155797</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.1171127197772476</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.12782619104379569</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.17371953196697132</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.24524115863881962</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.3302067695694289</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.43277773184398072</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.55017783047409574</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.66839938854324343</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.77736347144939966</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.85216100823247387</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.91926977899459761</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.95554810766148401</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.96740326760549356</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.95248780396916277</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.90842586639577949</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.82928489796612925</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.74486791168752042</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.63262711162410201</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.51939914229838391</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.395817593538898</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.2927815849329144</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.21246606788463041</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.13968895236264731</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.11899170769139168</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.11732368854773158</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.14877627311873093</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.21591131530151458</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.29420486810201163</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.4014093055057365</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.49571537561436008</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-DE82-451E-8BB6-61DDB4CE8779}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>60°</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$A$2:$A$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="40"/>
+                <c:pt idx="0">
+                  <c:v>-375</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-355.76923076923089</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-336.53846153846177</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-317.30769230769226</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-298.07692307692315</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-278.84615384615398</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-259.61538461538447</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-240.38461538461536</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-221.15384615384625</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-201.92307692307674</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-182.69230769230762</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-163.46153846153851</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-144.2307692307694</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-124.99999999999987</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-105.76923076923075</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-86.538461538461632</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-67.307692307692491</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>-48.076923076923002</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>-28.846153846153836</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>-9.6153846153846363</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>9.615384615384599</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>28.846153846153836</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>48.076923076923002</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>67.307692307692491</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>86.538461538461632</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>105.76923076923075</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>124.99999999999987</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>144.2307692307694</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>163.46153846153851</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>182.69230769230762</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>201.92307692307713</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>221.15384615384625</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>240.38461538461536</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>259.61538461538447</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>278.84615384615398</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>298.07692307692315</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>317.30769230769226</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>336.53846153846138</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>355.76923076923089</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>375</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$G$2:$G$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="40"/>
+                <c:pt idx="0">
+                  <c:v>0.47515892532059556</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5641977878897928</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.67063318110482106</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.76762404674184115</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.83722587362604151</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.8901282053996501</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.9117720348108268</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.90409268186286318</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.88461869375998392</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.82554717349158391</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.74413204200044247</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.64562774182018978</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.52481263531196842</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.41894315617886846</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.31385085112822736</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.2240017913198894</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.15968455740166229</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.11750195091251814</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.12030477228748991</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.16424059109149305</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.24213634964319769</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.32167300652446434</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.42090852402475365</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.53441000160555607</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.63781032513298574</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.7439389177856125</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.81449148765844648</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.87804012023243083</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.89726303452048761</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.90442226210843246</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.88812624155010322</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.84936005551942106</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.76325977238745557</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.66466106524988533</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.56718392997416189</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.45273523325689602</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.3495421271835002</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.26083667906725333</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.18832462495737248</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-DE82-451E-8BB6-61DDB4CE8779}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>120°</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$A$2:$A$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="40"/>
+                <c:pt idx="0">
+                  <c:v>-375</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-355.76923076923089</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-336.53846153846177</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-317.30769230769226</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-298.07692307692315</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-278.84615384615398</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-259.61538461538447</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-240.38461538461536</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-221.15384615384625</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-201.92307692307674</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-182.69230769230762</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-163.46153846153851</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-144.2307692307694</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-124.99999999999987</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-105.76923076923075</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-86.538461538461632</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-67.307692307692491</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>-48.076923076923002</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>-28.846153846153836</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>-9.6153846153846363</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>9.615384615384599</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>28.846153846153836</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>48.076923076923002</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>67.307692307692491</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>86.538461538461632</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>105.76923076923075</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>124.99999999999987</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>144.2307692307694</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>163.46153846153851</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>182.69230769230762</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>201.92307692307713</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>221.15384615384625</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>240.38461538461536</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>259.61538461538447</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>278.84615384615398</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>298.07692307692315</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>317.30769230769226</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>336.53846153846138</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>355.76923076923089</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>375</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$H$2:$H$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="40"/>
+                <c:pt idx="0">
+                  <c:v>0.21598096613103299</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.14199374122804567</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.11159906168881908</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.10879361150579403</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.13326168784216436</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.19934020425049925</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.28991148207968181</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.42610958981813207</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.54238077688695985</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.65657017127297401</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.77302545558493097</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.85980501636591344</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.93151065408405176</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.98332879359848924</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.99369771054493095</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.98646721705238272</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.94399074252693149</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.86782644745214887</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.78980273471944995</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.6835394074287896</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.57810981239384285</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.4614650428531426</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.35335015080714161</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.23294542726767639</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.17293283192807324</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.11906814654149855</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.1111922336865592</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.14130946282119283</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.18323461042576311</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.28716843902422512</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.38650554913896273</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.50598186594826533</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.62164935963002055</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.73681715266188763</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.83926692217818122</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.91424072901527775</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.96412178862512066</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.99304984761129556</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.96404025657471093</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-DE82-451E-8BB6-61DDB4CE8779}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="354102496"/>
+        <c:axId val="239759648"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="354102496"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="400"/>
+          <c:min val="-400"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Pockels cell</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> voltage (V)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="239759648"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="50"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="239759648"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1.05"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="354102496"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1953,20 +3271,536 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>273661</xdr:colOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>108805</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>81328</xdr:rowOff>
+      <xdr:rowOff>127122</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>150993</xdr:colOff>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>599767</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>96039</xdr:rowOff>
+      <xdr:rowOff>141833</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1986,6 +3820,44 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>393822</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>183172</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>271153</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>5552</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D952B54F-F224-41F9-B1A6-87A18A8237D0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3651,7 +5523,7 @@
         <v>-375</v>
       </c>
       <c r="B20">
-        <f t="shared" ref="B20:AN21" si="2">B1*375</f>
+        <f t="shared" ref="B20:AN20" si="2">B1*375</f>
         <v>-355.76923076923089</v>
       </c>
       <c r="C20">
@@ -3936,15 +5808,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BD7A667-8C18-4D1C-ACFB-41A167CE9F75}">
-  <dimension ref="A1:D41"/>
+  <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="104" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" zoomScale="105" workbookViewId="0">
+      <selection activeCell="T22" sqref="T22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3958,7 +5830,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>-375</v>
       </c>
@@ -3971,8 +5843,20 @@
       <c r="D2">
         <v>0.58931037524444274</v>
       </c>
+      <c r="F2">
+        <f>0.9*(B2-MIN($B:$D))/(MAX($B:$D)-MIN($B:$D)) + 0.1</f>
+        <v>0.93460750664971581</v>
+      </c>
+      <c r="G2">
+        <f t="shared" ref="G2:H17" si="0">0.9*(C2-MIN($B:$D))/(MAX($B:$D)-MIN($B:$D)) + 0.1</f>
+        <v>0.47515892532059556</v>
+      </c>
+      <c r="H2">
+        <f t="shared" si="0"/>
+        <v>0.21598096613103299</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>-355.76923076923089</v>
       </c>
@@ -3985,8 +5869,20 @@
       <c r="D3">
         <v>0.55055393653635998</v>
       </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F41" si="1">0.9*(B3-MIN($B:$D))/(MAX($B:$D)-MIN($B:$D)) + 0.1</f>
+        <v>0.88921086627950874</v>
+      </c>
+      <c r="G3">
+        <f t="shared" si="0"/>
+        <v>0.5641977878897928</v>
+      </c>
+      <c r="H3">
+        <f t="shared" si="0"/>
+        <v>0.14199374122804567</v>
+      </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>-336.53846153846177</v>
       </c>
@@ -3999,8 +5895,20 @@
       <c r="D4">
         <v>0.53463241040589027</v>
       </c>
+      <c r="F4">
+        <f t="shared" si="1"/>
+        <v>0.80895359754091334</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="0"/>
+        <v>0.67063318110482106</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="0"/>
+        <v>0.11159906168881908</v>
+      </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>-317.30769230769226</v>
       </c>
@@ -4013,8 +5921,20 @@
       <c r="D5">
         <v>0.53316284240669098</v>
       </c>
+      <c r="F5">
+        <f t="shared" si="1"/>
+        <v>0.70382335956106368</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="0"/>
+        <v>0.76762404674184115</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="0"/>
+        <v>0.10879361150579403</v>
+      </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>-298.07692307692315</v>
       </c>
@@ -4027,8 +5947,20 @@
       <c r="D6">
         <v>0.54597985915625336</v>
       </c>
+      <c r="F6">
+        <f t="shared" si="1"/>
+        <v>0.5970662829615776</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="0"/>
+        <v>0.83722587362604151</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="0"/>
+        <v>0.13326168784216436</v>
+      </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>-278.84615384615398</v>
       </c>
@@ -4041,8 +5973,20 @@
       <c r="D7">
         <v>0.58059351001906967</v>
       </c>
+      <c r="F7">
+        <f t="shared" si="1"/>
+        <v>0.48301577109411531</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="0"/>
+        <v>0.8901282053996501</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="0"/>
+        <v>0.19934020425049925</v>
+      </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>-259.61538461538447</v>
       </c>
@@ -4055,8 +5999,20 @@
       <c r="D8">
         <v>0.62803710832272386</v>
       </c>
+      <c r="F8">
+        <f t="shared" si="1"/>
+        <v>0.38254029659280375</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>0.9117720348108268</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="0"/>
+        <v>0.28991148207968181</v>
+      </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>-240.38461538461536</v>
       </c>
@@ -4069,8 +6025,20 @@
       <c r="D9">
         <v>0.69938123052278456</v>
       </c>
+      <c r="F9">
+        <f t="shared" si="1"/>
+        <v>0.27416444981191507</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="0"/>
+        <v>0.90409268186286318</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="0"/>
+        <v>0.42610958981813207</v>
+      </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>-221.15384615384625</v>
       </c>
@@ -4083,8 +6051,20 @@
       <c r="D10">
         <v>0.76028711178887731</v>
       </c>
+      <c r="F10">
+        <f t="shared" si="1"/>
+        <v>0.19902187846008601</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>0.88461869375998392</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="0"/>
+        <v>0.54238077688695985</v>
+      </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>-201.92307692307674</v>
       </c>
@@ -4097,8 +6077,20 @@
       <c r="D11">
         <v>0.82010249573438276</v>
       </c>
+      <c r="F11">
+        <f t="shared" si="1"/>
+        <v>0.14272764542155797</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="0"/>
+        <v>0.82554717349158391</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="0"/>
+        <v>0.65657017127297401</v>
+      </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>-182.69230769230762</v>
       </c>
@@ -4111,8 +6103,20 @@
       <c r="D12">
         <v>0.88110481193946699</v>
       </c>
+      <c r="F12">
+        <f t="shared" si="1"/>
+        <v>0.1171127197772476</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>0.74413204200044247</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="0"/>
+        <v>0.77302545558493097</v>
+      </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>-163.46153846153851</v>
       </c>
@@ -4125,8 +6129,20 @@
       <c r="D13">
         <v>0.92656220992854454</v>
       </c>
+      <c r="F13">
+        <f t="shared" si="1"/>
+        <v>0.12782619104379569</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="0"/>
+        <v>0.64562774182018978</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="0"/>
+        <v>0.85980501636591344</v>
+      </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>-144.2307692307694</v>
       </c>
@@ -4139,8 +6155,20 @@
       <c r="D14">
         <v>0.96412349374329687</v>
       </c>
+      <c r="F14">
+        <f t="shared" si="1"/>
+        <v>0.17371953196697132</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="0"/>
+        <v>0.52481263531196842</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="0"/>
+        <v>0.93151065408405176</v>
+      </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>-124.99999999999987</v>
       </c>
@@ -4153,8 +6181,20 @@
       <c r="D15">
         <v>0.99126718714025097</v>
       </c>
+      <c r="F15">
+        <f t="shared" si="1"/>
+        <v>0.24524115863881962</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="0"/>
+        <v>0.41894315617886846</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="0"/>
+        <v>0.98332879359848924</v>
+      </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>-105.76923076923075</v>
       </c>
@@ -4167,8 +6207,20 @@
       <c r="D16">
         <v>0.99669869635864505</v>
       </c>
+      <c r="F16">
+        <f t="shared" si="1"/>
+        <v>0.3302067695694289</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="0"/>
+        <v>0.31385085112822736</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="0"/>
+        <v>0.99369771054493095</v>
+      </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>-86.538461538461632</v>
       </c>
@@ -4181,8 +6233,20 @@
       <c r="D17">
         <v>0.99291117522590122</v>
       </c>
+      <c r="F17">
+        <f t="shared" si="1"/>
+        <v>0.43277773184398072</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="0"/>
+        <v>0.2240017913198894</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="0"/>
+        <v>0.98646721705238272</v>
+      </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>-67.307692307692491</v>
       </c>
@@ -4195,8 +6259,20 @@
       <c r="D18">
         <v>0.9706608896713389</v>
       </c>
+      <c r="F18">
+        <f t="shared" si="1"/>
+        <v>0.55017783047409574</v>
+      </c>
+      <c r="G18">
+        <f t="shared" ref="G18:G41" si="2">0.9*(C18-MIN($B:$D))/(MAX($B:$D)-MIN($B:$D)) + 0.1</f>
+        <v>0.15968455740166229</v>
+      </c>
+      <c r="H18">
+        <f t="shared" ref="H18:H41" si="3">0.9*(D18-MIN($B:$D))/(MAX($B:$D)-MIN($B:$D)) + 0.1</f>
+        <v>0.94399074252693149</v>
+      </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>-48.076923076923002</v>
       </c>
@@ -4209,8 +6285,20 @@
       <c r="D19">
         <v>0.93076404480817987</v>
       </c>
+      <c r="F19">
+        <f t="shared" si="1"/>
+        <v>0.66839938854324343</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="2"/>
+        <v>0.11750195091251814</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="3"/>
+        <v>0.86782644745214887</v>
+      </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>-28.846153846153836</v>
       </c>
@@ -4223,8 +6311,20 @@
       <c r="D20">
         <v>0.88989318846417054</v>
       </c>
+      <c r="F20">
+        <f t="shared" si="1"/>
+        <v>0.77736347144939966</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="2"/>
+        <v>0.1</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="3"/>
+        <v>0.78980273471944995</v>
+      </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>-9.6153846153846363</v>
       </c>
@@ -4237,8 +6337,20 @@
       <c r="D21">
         <v>0.83422968525185948</v>
       </c>
+      <c r="F21">
+        <f t="shared" si="1"/>
+        <v>0.85216100823247387</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="2"/>
+        <v>0.12030477228748991</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="3"/>
+        <v>0.6835394074287896</v>
+      </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>9.615384615384599</v>
       </c>
@@ -4251,8 +6363,20 @@
       <c r="D22">
         <v>0.7790029127469088</v>
       </c>
+      <c r="F22">
+        <f t="shared" si="1"/>
+        <v>0.91926977899459761</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="2"/>
+        <v>0.16424059109149305</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="3"/>
+        <v>0.57810981239384285</v>
+      </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>28.846153846153836</v>
       </c>
@@ -4265,8 +6389,20 @@
       <c r="D23">
         <v>0.71790133923539767</v>
       </c>
+      <c r="F23">
+        <f t="shared" si="1"/>
+        <v>0.95554810766148401</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="2"/>
+        <v>0.24213634964319769</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="3"/>
+        <v>0.4614650428531426</v>
+      </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>48.076923076923002</v>
       </c>
@@ -4279,8 +6415,20 @@
       <c r="D24">
         <v>0.6612679380974853</v>
       </c>
+      <c r="F24">
+        <f t="shared" si="1"/>
+        <v>0.96740326760549356</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="2"/>
+        <v>0.32167300652446434</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="3"/>
+        <v>0.35335015080714161</v>
+      </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>67.307692307692491</v>
       </c>
@@ -4293,8 +6441,20 @@
       <c r="D25">
         <v>0.59819680258537988</v>
       </c>
+      <c r="F25">
+        <f t="shared" si="1"/>
+        <v>0.95248780396916277</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="2"/>
+        <v>0.42090852402475365</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="3"/>
+        <v>0.23294542726767639</v>
+      </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>86.538461538461632</v>
       </c>
@@ -4307,8 +6467,20 @@
       <c r="D26">
         <v>0.56676063943637667</v>
       </c>
+      <c r="F26">
+        <f t="shared" si="1"/>
+        <v>0.90842586639577949</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="2"/>
+        <v>0.53441000160555607</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="3"/>
+        <v>0.17293283192807324</v>
+      </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>105.76923076923075</v>
       </c>
@@ -4321,8 +6493,20 @@
       <c r="D27">
         <v>0.53854491191784593</v>
       </c>
+      <c r="F27">
+        <f t="shared" si="1"/>
+        <v>0.82928489796612925</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="2"/>
+        <v>0.63781032513298574</v>
+      </c>
+      <c r="H27">
+        <f t="shared" si="3"/>
+        <v>0.11906814654149855</v>
+      </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>124.99999999999987</v>
       </c>
@@ -4335,8 +6519,20 @@
       <c r="D28">
         <v>0.53441930328428933</v>
       </c>
+      <c r="F28">
+        <f t="shared" si="1"/>
+        <v>0.74486791168752042</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="2"/>
+        <v>0.7439389177856125</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="3"/>
+        <v>0.1111922336865592</v>
+      </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>144.2307692307694</v>
       </c>
@@ -4349,8 +6545,20 @@
       <c r="D29">
         <v>0.5501954936542377</v>
       </c>
+      <c r="F29">
+        <f t="shared" si="1"/>
+        <v>0.63262711162410201</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="2"/>
+        <v>0.81449148765844648</v>
+      </c>
+      <c r="H29">
+        <f t="shared" si="3"/>
+        <v>0.14130946282119283</v>
+      </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>163.46153846153851</v>
       </c>
@@ -4363,8 +6571,20 @@
       <c r="D30">
         <v>0.57215697978369306</v>
       </c>
+      <c r="F30">
+        <f t="shared" si="1"/>
+        <v>0.51939914229838391</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="2"/>
+        <v>0.87804012023243083</v>
+      </c>
+      <c r="H30">
+        <f t="shared" si="3"/>
+        <v>0.18323461042576311</v>
+      </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>182.69230769230762</v>
       </c>
@@ -4377,8 +6597,20 @@
       <c r="D31">
         <v>0.62660023080512761</v>
       </c>
+      <c r="F31">
+        <f t="shared" si="1"/>
+        <v>0.395817593538898</v>
+      </c>
+      <c r="G31">
+        <f t="shared" si="2"/>
+        <v>0.89726303452048761</v>
+      </c>
+      <c r="H31">
+        <f t="shared" si="3"/>
+        <v>0.28716843902422512</v>
+      </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>201.92307692307713</v>
       </c>
@@ -4391,8 +6623,20 @@
       <c r="D32">
         <v>0.67863560075781859</v>
       </c>
+      <c r="F32">
+        <f t="shared" si="1"/>
+        <v>0.2927815849329144</v>
+      </c>
+      <c r="G32">
+        <f t="shared" si="2"/>
+        <v>0.90442226210843246</v>
+      </c>
+      <c r="H32">
+        <f t="shared" si="3"/>
+        <v>0.38650554913896273</v>
+      </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>221.15384615384625</v>
       </c>
@@ -4405,8 +6649,20 @@
       <c r="D33">
         <v>0.74122041260281935</v>
       </c>
+      <c r="F33">
+        <f t="shared" si="1"/>
+        <v>0.21246606788463041</v>
+      </c>
+      <c r="G33">
+        <f t="shared" si="2"/>
+        <v>0.88812624155010322</v>
+      </c>
+      <c r="H33">
+        <f t="shared" si="3"/>
+        <v>0.50598186594826533</v>
+      </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>240.38461538461536</v>
       </c>
@@ -4419,8 +6675,20 @@
       <c r="D34">
         <v>0.8018100635225891</v>
       </c>
+      <c r="F34">
+        <f t="shared" si="1"/>
+        <v>0.13968895236264731</v>
+      </c>
+      <c r="G34">
+        <f t="shared" si="2"/>
+        <v>0.84936005551942106</v>
+      </c>
+      <c r="H34">
+        <f t="shared" si="3"/>
+        <v>0.62164935963002055</v>
+      </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>259.61538461538447</v>
       </c>
@@ -4433,8 +6701,20 @@
       <c r="D35">
         <v>0.86213795820491146</v>
       </c>
+      <c r="F35">
+        <f t="shared" si="1"/>
+        <v>0.11899170769139168</v>
+      </c>
+      <c r="G35">
+        <f t="shared" si="2"/>
+        <v>0.76325977238745557</v>
+      </c>
+      <c r="H35">
+        <f t="shared" si="3"/>
+        <v>0.73681715266188763</v>
+      </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>278.84615384615398</v>
       </c>
@@ -4447,8 +6727,20 @@
       <c r="D36">
         <v>0.91580382036046204</v>
       </c>
+      <c r="F36">
+        <f t="shared" si="1"/>
+        <v>0.11732368854773158</v>
+      </c>
+      <c r="G36">
+        <f t="shared" si="2"/>
+        <v>0.66466106524988533</v>
+      </c>
+      <c r="H36">
+        <f t="shared" si="3"/>
+        <v>0.83926692217818122</v>
+      </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>298.07692307692315</v>
       </c>
@@ -4461,8 +6753,20 @@
       <c r="D37">
         <v>0.95507705642524987</v>
       </c>
+      <c r="F37">
+        <f t="shared" si="1"/>
+        <v>0.14877627311873093</v>
+      </c>
+      <c r="G37">
+        <f t="shared" si="2"/>
+        <v>0.56718392997416189</v>
+      </c>
+      <c r="H37">
+        <f t="shared" si="3"/>
+        <v>0.91424072901527775</v>
+      </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>317.30769230769226</v>
       </c>
@@ -4475,8 +6779,20 @@
       <c r="D38">
         <v>0.98120605683035955</v>
       </c>
+      <c r="F38">
+        <f t="shared" si="1"/>
+        <v>0.21591131530151458</v>
+      </c>
+      <c r="G38">
+        <f t="shared" si="2"/>
+        <v>0.45273523325689602</v>
+      </c>
+      <c r="H38">
+        <f t="shared" si="3"/>
+        <v>0.96412178862512066</v>
+      </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>336.53846153846138</v>
       </c>
@@ -4489,8 +6805,20 @@
       <c r="D39">
         <v>1</v>
       </c>
+      <c r="F39">
+        <f t="shared" si="1"/>
+        <v>0.29420486810201163</v>
+      </c>
+      <c r="G39">
+        <f t="shared" si="2"/>
+        <v>0.3495421271835002</v>
+      </c>
+      <c r="H39">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>355.76923076923089</v>
       </c>
@@ -4503,8 +6831,20 @@
       <c r="D40">
         <v>0.9963593288514625</v>
       </c>
+      <c r="F40">
+        <f t="shared" si="1"/>
+        <v>0.4014093055057365</v>
+      </c>
+      <c r="G40">
+        <f t="shared" si="2"/>
+        <v>0.26083667906725333</v>
+      </c>
+      <c r="H40">
+        <f t="shared" si="3"/>
+        <v>0.99304984761129556</v>
+      </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>375</v>
       </c>
@@ -4516,6 +6856,18 @@
       </c>
       <c r="D41">
         <v>0.9811633482152089</v>
+      </c>
+      <c r="F41">
+        <f t="shared" si="1"/>
+        <v>0.49571537561436008</v>
+      </c>
+      <c r="G41">
+        <f t="shared" si="2"/>
+        <v>0.18832462495737248</v>
+      </c>
+      <c r="H41">
+        <f t="shared" si="3"/>
+        <v>0.96404025657471093</v>
       </c>
     </row>
   </sheetData>

</xml_diff>